<commit_message>
cree la variable estado pedido en la base de datos y a la hora de crearse se vea como pendiente
</commit_message>
<xml_diff>
--- a/paquetes.xlsx
+++ b/paquetes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,68 +452,46 @@
           <t>Dimensiones</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>estado pedido</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>prueba</t>
+          <t>prueba 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20 kg</t>
+          <t>40 kg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dimensionado</t>
+          <t>basico</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>arroz,  papa,  yuca</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>alimentos</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>20 kg</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>dimensionado</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>20</t>
+          <t>20x20x20</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>pendiente</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Siguiendo con la gestion de usuarios
</commit_message>
<xml_diff>
--- a/paquetes.xlsx
+++ b/paquetes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Taladro</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>50 kg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>basico</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1 Taladro</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Herramientas electronicas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10x10x10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>pendiente</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
solucion de problemas con la variable usuario
</commit_message>
<xml_diff>
--- a/paquetes.xlsx
+++ b/paquetes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,57 +424,99 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Creador</t>
+          <t>Nombre</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Nombre</t>
+          <t>Precio</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Precio</t>
+          <t>Peso</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>Tipo</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Tipo</t>
+          <t>Contenido</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Contenido</t>
+          <t>Categoría</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Categoría</t>
+          <t>Dimensiones</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Dimensiones</t>
+          <t>Estado pedido</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>estado pedido</t>
+          <t>Direccion</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Direccion</t>
+          <t>Domiciliario</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Domiciliario</t>
+          <t>Usuario</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>taladro</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10000 $</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20 kg</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>basico</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>taladro</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>herramientas</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10x10x10</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>pendiente</t>
         </is>
       </c>
     </row>

</xml_diff>